<commit_message>
Enhance URL fetching logic for product details extraction: Improve the `fetch_product_from_url` function by adding detailed logging for extracted ingredients and text, implementing robust fallback mechanisms for product name and brand extraction, and refining the caching logic to ensure data integrity. This update enhances error handling and provides clearer feedback during the scraping process, improving overall functionality and user experience.
</commit_message>
<xml_diff>
--- a/endpoint_timing.xlsx
+++ b/endpoint_timing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,74 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-01-09T12:23:37.609996+00:00</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>/api/inspiration-boards/products/6960ee6adfdda64b2c01ef32</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Inspiration Boards</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1571</v>
+      </c>
+      <c r="F2" t="n">
+        <v>200</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6925b1e37b5978266363464e</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-09T12:23:37.759328+00:00</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>/api/inspiration-boards/boards/6960eb294ad6a4df36746c2b</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Inspiration Boards</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0946</v>
+      </c>
+      <c r="F3" t="n">
+        <v>200</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>6925b1e37b5978266363464e</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance platform handling in product logic: Introduce a new function to filter platform details for list display, ensuring only essential fields (title, logo_url, platform_display_name) are included. Update product summary formatting to incorporate filtered platform data. Additionally, expand platform domain and display name mappings, and implement a fallback mechanism for favicon URLs when S3 logos are unavailable, improving overall platform integration and user experience.
</commit_message>
<xml_diff>
--- a/endpoint_timing.xlsx
+++ b/endpoint_timing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,108 @@
       </c>
       <c r="H3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-09T13:27:54.321641+00:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>/api/inspiration-boards/boards/6960eb294ad6a4df36746c2b</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Inspiration Boards</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1207</v>
+      </c>
+      <c r="F4" t="n">
+        <v>200</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6925b1e37b5978266363464e</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-09T13:27:58.901902+00:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>/api/inspiration-boards/boards</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Inspiration Boards</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0.4167</v>
+      </c>
+      <c r="F5" t="n">
+        <v>200</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6925b1e37b5978266363464e</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-09T13:27:59.273055+00:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>/api/inspiration-boards/boards</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Inspiration Boards</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3671</v>
+      </c>
+      <c r="F6" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6925b1e37b5978266363464e</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>